<commit_message>
successfully implemented upload dynamic records funtion
</commit_message>
<xml_diff>
--- a/app/files/Part-Time Lecturer Requisition Form - template new.xlsx
+++ b/app/files/Part-Time Lecturer Requisition Form - template new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\k\Main\Capstone Project\CoursePDF Extractor\Capstone-Project\app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88883402-09B9-4077-8883-6F6CAB78F360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A523E8C1-BB0D-46D8-80B4-BCEFDD252CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,9 +216,6 @@
     <t>Approved by Academic Director</t>
   </si>
   <si>
-    <t>____________________</t>
-  </si>
-  <si>
     <t>Name:  Asihvini Govinda Pilay</t>
   </si>
   <si>
@@ -240,10 +237,13 @@
     <t>1. This form applicable to both new and regular part-time lecturers.</t>
   </si>
   <si>
-    <t>2. Any part-time lecturer commencement date start after the 10th of the month, their payment can only be process from following month onwards.</t>
-  </si>
-  <si>
     <t>3. Any changes of payment, HOP must notify HR immediately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Any part-time lecturer commencement date start after the 10th of the month, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    their payment can only be process from following month onwards.</t>
   </si>
 </sst>
 </file>
@@ -304,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -426,14 +426,60 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -441,36 +487,12 @@
       <left style="thin">
         <color rgb="FFC6C6C6"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -549,10 +571,7 @@
     <xf numFmtId="3" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -561,7 +580,7 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -580,44 +599,34 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,44 +933,45 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L77"/>
+  <dimension ref="A3:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:K20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-    </row>
-    <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -975,7 +985,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
         <v>1</v>
@@ -991,7 +1001,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1000,13 +1010,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1020,7 +1029,7 @@
       <c r="K9" s="10"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
         <v>5</v>
@@ -1032,7 +1041,7 @@
       <c r="I10" s="15"/>
       <c r="L10" s="16"/>
     </row>
-    <row r="11" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="5" t="s">
         <v>7</v>
@@ -1040,22 +1049,22 @@
       <c r="D11" s="17"/>
       <c r="L11" s="16"/>
     </row>
-    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="L12" s="16"/>
     </row>
-    <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="L13" s="16"/>
     </row>
-    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="L14" s="16"/>
     </row>
-    <row r="15" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="18" t="s">
         <v>9</v>
@@ -1077,7 +1086,7 @@
       </c>
       <c r="L15" s="16"/>
     </row>
-    <row r="16" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="18" t="s">
         <v>13</v>
@@ -1099,7 +1108,7 @@
       </c>
       <c r="L16" s="16"/>
     </row>
-    <row r="17" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="18" t="s">
         <v>14</v>
@@ -1121,7 +1130,7 @@
       </c>
       <c r="L17" s="16"/>
     </row>
-    <row r="18" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="18" t="s">
         <v>15</v>
@@ -1143,16 +1152,16 @@
       </c>
       <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="L19" s="16"/>
     </row>
-    <row r="20" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="45"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="21"/>
       <c r="E20" s="22" t="s">
         <v>17</v>
@@ -1165,43 +1174,43 @@
       <c r="H20" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="46">
+      <c r="I20" s="44"/>
+      <c r="J20" s="45">
         <f>D20*G20</f>
         <v>0</v>
       </c>
-      <c r="K20" s="47"/>
+      <c r="K20" s="46"/>
       <c r="L20" s="16"/>
     </row>
     <row r="21" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="28"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="23" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="36"/>
       <c r="L23" s="18"/>
     </row>
-    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
+    <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
       <c r="L24" s="18"/>
     </row>
-    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="L25" s="18"/>
     </row>
     <row r="26" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -1211,512 +1220,489 @@
       <c r="E26" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="29" t="s">
         <v>22</v>
       </c>
       <c r="L26" s="18"/>
     </row>
-    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="I27" s="4"/>
       <c r="L27" s="18"/>
     </row>
     <row r="28" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="I28" s="30" t="s">
+      <c r="B28" s="40"/>
+      <c r="C28" s="34"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="I28" s="43"/>
+      <c r="L28" s="18"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B29" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="L28" s="18"/>
-    </row>
-    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="18" t="s">
+      <c r="E29" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="I29" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="18"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="18" t="s">
+      <c r="E30" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="I30" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="30" t="s">
+      <c r="L30" s="18"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B32" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L30" s="18"/>
-    </row>
-    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L31" s="18"/>
-    </row>
-    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="18" t="s">
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B33" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="L32" s="18"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B33" s="36" t="s">
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="18"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B34" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="18"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="18"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="30"/>
+      <c r="B36" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="18"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B34" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="18"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B35" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="18"/>
-    </row>
-    <row r="36" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="31"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="31"/>
-    </row>
-    <row r="37" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="30"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
+      <c r="B37" s="32"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
-      <c r="G37" s="30"/>
+      <c r="G37" s="29"/>
       <c r="H37" s="18"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
       <c r="K37" s="18"/>
       <c r="L37" s="18"/>
     </row>
-    <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="34"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="33"/>
       <c r="H38" s="5"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="33"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="32"/>
       <c r="L38" s="18"/>
     </row>
-    <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="33"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="18"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="33"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="32"/>
       <c r="L39" s="18"/>
     </row>
-    <row r="40" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="33"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="32"/>
       <c r="L40" s="18"/>
     </row>
-    <row r="41" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="34"/>
-      <c r="K41" s="33"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="32"/>
       <c r="L41" s="18"/>
     </row>
-    <row r="42" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="33"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="32"/>
       <c r="L42" s="18"/>
     </row>
-    <row r="43" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="33"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="30"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="29"/>
       <c r="H43" s="18"/>
-      <c r="I43" s="32"/>
+      <c r="I43" s="31"/>
       <c r="J43" s="20"/>
-      <c r="K43" s="33"/>
+      <c r="K43" s="32"/>
       <c r="L43" s="18"/>
     </row>
-    <row r="44" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
-      <c r="C44" s="33"/>
+      <c r="C44" s="32"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="30"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="29"/>
       <c r="H44" s="18"/>
-      <c r="I44" s="32"/>
+      <c r="I44" s="31"/>
       <c r="J44" s="20"/>
-      <c r="K44" s="33"/>
+      <c r="K44" s="32"/>
       <c r="L44" s="18"/>
     </row>
-    <row r="45" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
-      <c r="C45" s="33"/>
+      <c r="C45" s="32"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="30"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="29"/>
       <c r="H45" s="18"/>
-      <c r="I45" s="32"/>
+      <c r="I45" s="31"/>
       <c r="J45" s="20"/>
-      <c r="K45" s="33"/>
+      <c r="K45" s="32"/>
       <c r="L45" s="18"/>
     </row>
-    <row r="46" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
-      <c r="C46" s="33"/>
+      <c r="C46" s="32"/>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="30"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="29"/>
       <c r="H46" s="18"/>
-      <c r="I46" s="32"/>
+      <c r="I46" s="31"/>
       <c r="J46" s="20"/>
-      <c r="K46" s="33"/>
+      <c r="K46" s="32"/>
       <c r="L46" s="18"/>
     </row>
-    <row r="47" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="33"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="32"/>
       <c r="L47" s="18"/>
     </row>
-    <row r="48" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="18"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="5"/>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="32"/>
+      <c r="G48" s="31"/>
       <c r="H48" s="18"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="38"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="48"/>
       <c r="L48" s="18"/>
     </row>
-    <row r="49" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
+      <c r="B49" s="5"/>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
-      <c r="G49" s="30"/>
+      <c r="G49" s="29"/>
       <c r="H49" s="18"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
-    <row r="50" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="31"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="33"/>
-      <c r="L50" s="31"/>
-    </row>
-    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="30"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="30"/>
+    </row>
+    <row r="51" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
-      <c r="B51" s="5"/>
+      <c r="B51" s="32"/>
       <c r="C51" s="18"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="34"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="33"/>
       <c r="H51" s="5"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="33"/>
-      <c r="L51" s="31"/>
-    </row>
-    <row r="52" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I51" s="29"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="30"/>
+    </row>
+    <row r="52" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="5"/>
-      <c r="C52" s="33"/>
+      <c r="C52" s="32"/>
       <c r="D52" s="18"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="33"/>
-      <c r="L52" s="31"/>
-    </row>
-    <row r="53" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="32"/>
+      <c r="L52" s="30"/>
+    </row>
+    <row r="53" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="34"/>
-      <c r="K53" s="33"/>
-      <c r="L53" s="31"/>
-    </row>
-    <row r="54" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="5"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="32"/>
+      <c r="L53" s="30"/>
+    </row>
+    <row r="54" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="33"/>
-      <c r="L54" s="31"/>
-    </row>
-    <row r="55" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="32"/>
+      <c r="L54" s="30"/>
+    </row>
+    <row r="55" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="18"/>
-      <c r="B55" s="33"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="34"/>
-      <c r="K55" s="33"/>
-      <c r="L55" s="31"/>
-    </row>
-    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="5"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="32"/>
+      <c r="L55" s="30"/>
+    </row>
+    <row r="56" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="33"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="30"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="29"/>
       <c r="H56" s="18"/>
-      <c r="I56" s="32"/>
+      <c r="I56" s="31"/>
       <c r="J56" s="20"/>
-      <c r="K56" s="33"/>
-      <c r="L56" s="31"/>
-    </row>
-    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K56" s="32"/>
+      <c r="L56" s="30"/>
+    </row>
+    <row r="57" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
       <c r="B57" s="18"/>
-      <c r="C57" s="33"/>
+      <c r="C57" s="32"/>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="30"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="29"/>
       <c r="H57" s="18"/>
-      <c r="I57" s="32"/>
+      <c r="I57" s="31"/>
       <c r="J57" s="20"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="31"/>
-    </row>
-    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K57" s="32"/>
+      <c r="L57" s="30"/>
+    </row>
+    <row r="58" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="18"/>
       <c r="B58" s="18"/>
-      <c r="C58" s="33"/>
+      <c r="C58" s="32"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="30"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="29"/>
       <c r="H58" s="18"/>
-      <c r="I58" s="32"/>
+      <c r="I58" s="31"/>
       <c r="J58" s="20"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="31"/>
-    </row>
-    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K58" s="32"/>
+      <c r="L58" s="30"/>
+    </row>
+    <row r="59" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="18"/>
-      <c r="C59" s="33"/>
+      <c r="C59" s="32"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="30"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="29"/>
       <c r="H59" s="18"/>
-      <c r="I59" s="32"/>
+      <c r="I59" s="31"/>
       <c r="J59" s="20"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="31"/>
-    </row>
-    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K59" s="32"/>
+      <c r="L59" s="30"/>
+    </row>
+    <row r="60" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="31"/>
-    </row>
-    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="18"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="32"/>
+      <c r="L60" s="30"/>
+    </row>
+    <row r="61" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="5"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18"/>
-      <c r="G61" s="32"/>
+      <c r="G61" s="31"/>
       <c r="H61" s="18"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="38"/>
-      <c r="L61" s="31"/>
-    </row>
-    <row r="62" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I61" s="29"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="30"/>
+    </row>
+    <row r="62" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
-      <c r="B62" s="18"/>
+      <c r="B62" s="5"/>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
       <c r="F62" s="18"/>
-      <c r="G62" s="30"/>
+      <c r="G62" s="29"/>
       <c r="H62" s="18"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
       <c r="K62" s="18"/>
-      <c r="L62" s="31"/>
-    </row>
-    <row r="63" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="15.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="L62" s="30"/>
+    </row>
+    <row r="63" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B63" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="3">
+    <mergeCell ref="J61:K61"/>
     <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B48:C48"/>
     <mergeCell ref="J48:K48"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="B33:K33"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B35:K35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implemented remove temporary files after downloading.
</commit_message>
<xml_diff>
--- a/app/files/Part-Time Lecturer Requisition Form - template new.xlsx
+++ b/app/files/Part-Time Lecturer Requisition Form - template new.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\k\Main\Capstone Project\CoursePDF Extractor\Capstone-Project\app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A523E8C1-BB0D-46D8-80B4-BCEFDD252CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA99279-8C82-4A9E-8EF1-885ADB493410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Part-Time Lecturer Requisition Form</t>
   </si>
@@ -240,10 +240,7 @@
     <t>3. Any changes of payment, HOP must notify HR immediately.</t>
   </si>
   <si>
-    <t xml:space="preserve">2. Any part-time lecturer commencement date start after the 10th of the month, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    their payment can only be process from following month onwards.</t>
+    <t>2. Any part-time lecturer commencement date start after the 10th of the month, their payment can only be process from following month onwards.</t>
   </si>
 </sst>
 </file>
@@ -500,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -615,13 +612,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -933,45 +923,43 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A3:L63"/>
+  <dimension ref="A3:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.77734375" style="2" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="46"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -983,9 +971,8 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
         <v>1</v>
@@ -999,9 +986,8 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1010,12 +996,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1026,45 +1012,44 @@
       <c r="H9" s="10"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="18"/>
       <c r="H10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="15"/>
-      <c r="L10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="17"/>
-      <c r="L11" s="16"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="16"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
-      <c r="L14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="18" t="s">
         <v>9</v>
@@ -1084,9 +1069,9 @@
       <c r="J15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="18" t="s">
         <v>13</v>
@@ -1106,9 +1091,9 @@
       <c r="J16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="16"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="18" t="s">
         <v>14</v>
@@ -1128,9 +1113,9 @@
       <c r="J17" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="16"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="18" t="s">
         <v>15</v>
@@ -1150,13 +1135,13 @@
       <c r="J18" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="16"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K18" s="16"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
-      <c r="L19" s="16"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K19" s="16"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="41" t="s">
         <v>16</v>
@@ -1179,10 +1164,9 @@
         <f>D20*G20</f>
         <v>0</v>
       </c>
-      <c r="K20" s="46"/>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="24"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
@@ -1193,27 +1177,26 @@
       <c r="H21" s="25"/>
       <c r="I21" s="26"/>
       <c r="J21" s="26"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="27"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K21" s="27"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G23" s="36" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="39"/>
       <c r="I23" s="37"/>
       <c r="J23" s="36"/>
-      <c r="L23" s="18"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
-      <c r="L24" s="18"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L25" s="18"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K24" s="18"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K25" s="18"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
         <v>20</v>
       </c>
@@ -1223,21 +1206,21 @@
       <c r="I26" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="L26" s="18"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K26" s="18"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="I27" s="4"/>
-      <c r="L27" s="18"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K27" s="18"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="40"/>
       <c r="C28" s="34"/>
       <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
+      <c r="F28" s="34"/>
       <c r="I28" s="43"/>
-      <c r="L28" s="18"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K28" s="18"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="18" t="s">
         <v>23</v>
       </c>
@@ -1247,9 +1230,9 @@
       <c r="I29" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K29" s="18"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="18" t="s">
         <v>25</v>
       </c>
@@ -1259,18 +1242,18 @@
       <c r="I30" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="L30" s="18"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L31" s="18"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K30" s="18"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K31" s="18"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L32" s="18"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K32" s="18"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="34" t="s">
         <v>29</v>
       </c>
@@ -1282,10 +1265,9 @@
       <c r="H33" s="34"/>
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="18"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K33" s="18"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="34" t="s">
         <v>31</v>
       </c>
@@ -1297,12 +1279,11 @@
       <c r="H34" s="34"/>
       <c r="I34" s="35"/>
       <c r="J34" s="35"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="18"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K34" s="18"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35" s="34"/>
       <c r="D35" s="34"/>
@@ -1312,14 +1293,11 @@
       <c r="H35" s="34"/>
       <c r="I35" s="35"/>
       <c r="J35" s="35"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="18"/>
-    </row>
-    <row r="36" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="30"/>
-      <c r="B36" s="34" t="s">
-        <v>30</v>
-      </c>
+      <c r="B36" s="32"/>
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
       <c r="E36" s="32"/>
@@ -1328,12 +1306,11 @@
       <c r="H36" s="32"/>
       <c r="I36" s="33"/>
       <c r="J36" s="33"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="30"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K36" s="30"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
-      <c r="B37" s="32"/>
+      <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
@@ -1343,11 +1320,10 @@
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
       <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="7"/>
       <c r="D38" s="32"/>
       <c r="E38" s="32"/>
@@ -1356,10 +1332,9 @@
       <c r="H38" s="5"/>
       <c r="I38" s="29"/>
       <c r="J38" s="33"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="18"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K38" s="18"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="5"/>
       <c r="C39" s="32"/>
@@ -1370,12 +1345,11 @@
       <c r="H39" s="32"/>
       <c r="I39" s="33"/>
       <c r="J39" s="33"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="18"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K39" s="18"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="32"/>
       <c r="D40" s="32"/>
       <c r="E40" s="32"/>
@@ -1384,12 +1358,11 @@
       <c r="H40" s="32"/>
       <c r="I40" s="33"/>
       <c r="J40" s="33"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="18"/>
-    </row>
-    <row r="41" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
-      <c r="B41" s="32"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="32"/>
       <c r="D41" s="32"/>
       <c r="E41" s="32"/>
@@ -1398,12 +1371,11 @@
       <c r="H41" s="32"/>
       <c r="I41" s="33"/>
       <c r="J41" s="33"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="18"/>
-    </row>
-    <row r="42" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K41" s="18"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="32"/>
       <c r="D42" s="32"/>
       <c r="E42" s="32"/>
@@ -1412,12 +1384,11 @@
       <c r="H42" s="32"/>
       <c r="I42" s="33"/>
       <c r="J42" s="33"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="18"/>
-    </row>
-    <row r="43" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K42" s="18"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
-      <c r="B43" s="32"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="32"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
@@ -1426,10 +1397,9 @@
       <c r="H43" s="18"/>
       <c r="I43" s="31"/>
       <c r="J43" s="20"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="18"/>
-    </row>
-    <row r="44" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K43" s="18"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="32"/>
@@ -1440,10 +1410,9 @@
       <c r="H44" s="18"/>
       <c r="I44" s="31"/>
       <c r="J44" s="20"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="18"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K44" s="18"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="32"/>
@@ -1454,10 +1423,9 @@
       <c r="H45" s="18"/>
       <c r="I45" s="31"/>
       <c r="J45" s="20"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="18"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K45" s="18"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="32"/>
@@ -1468,12 +1436,11 @@
       <c r="H46" s="18"/>
       <c r="I46" s="31"/>
       <c r="J46" s="20"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="18"/>
-    </row>
-    <row r="47" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K46" s="18"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
+      <c r="B47" s="32"/>
       <c r="C47" s="32"/>
       <c r="D47" s="32"/>
       <c r="E47" s="32"/>
@@ -1482,12 +1449,11 @@
       <c r="H47" s="32"/>
       <c r="I47" s="33"/>
       <c r="J47" s="33"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="18"/>
-    </row>
-    <row r="48" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K47" s="18"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="18"/>
-      <c r="B48" s="32"/>
+      <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
@@ -1495,13 +1461,12 @@
       <c r="G48" s="31"/>
       <c r="H48" s="18"/>
       <c r="I48" s="29"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="18"/>
-    </row>
-    <row r="49" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J48" s="8"/>
+      <c r="K48" s="18"/>
+    </row>
+    <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="18"/>
-      <c r="B49" s="5"/>
+      <c r="B49" s="18"/>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
@@ -1511,11 +1476,10 @@
       <c r="I49" s="29"/>
       <c r="J49" s="29"/>
       <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="30"/>
-      <c r="B50" s="18"/>
+      <c r="B50" s="32"/>
       <c r="C50" s="32"/>
       <c r="D50" s="32"/>
       <c r="E50" s="32"/>
@@ -1524,12 +1488,11 @@
       <c r="H50" s="32"/>
       <c r="I50" s="33"/>
       <c r="J50" s="33"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="30"/>
-    </row>
-    <row r="51" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K50" s="30"/>
+    </row>
+    <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
-      <c r="B51" s="32"/>
+      <c r="B51" s="5"/>
       <c r="C51" s="18"/>
       <c r="D51" s="32"/>
       <c r="E51" s="32"/>
@@ -1538,10 +1501,9 @@
       <c r="H51" s="5"/>
       <c r="I51" s="29"/>
       <c r="J51" s="33"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="30"/>
-    </row>
-    <row r="52" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K51" s="30"/>
+    </row>
+    <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="5"/>
       <c r="C52" s="32"/>
@@ -1552,12 +1514,11 @@
       <c r="H52" s="32"/>
       <c r="I52" s="33"/>
       <c r="J52" s="33"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="30"/>
-    </row>
-    <row r="53" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K52" s="30"/>
+    </row>
+    <row r="53" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
-      <c r="B53" s="5"/>
+      <c r="B53" s="32"/>
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>
       <c r="E53" s="32"/>
@@ -1566,12 +1527,11 @@
       <c r="H53" s="32"/>
       <c r="I53" s="33"/>
       <c r="J53" s="33"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="30"/>
-    </row>
-    <row r="54" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K53" s="30"/>
+    </row>
+    <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
-      <c r="B54" s="32"/>
+      <c r="B54" s="5"/>
       <c r="C54" s="32"/>
       <c r="D54" s="32"/>
       <c r="E54" s="32"/>
@@ -1580,12 +1540,11 @@
       <c r="H54" s="32"/>
       <c r="I54" s="33"/>
       <c r="J54" s="33"/>
-      <c r="K54" s="32"/>
-      <c r="L54" s="30"/>
-    </row>
-    <row r="55" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K54" s="30"/>
+    </row>
+    <row r="55" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="18"/>
-      <c r="B55" s="5"/>
+      <c r="B55" s="32"/>
       <c r="C55" s="32"/>
       <c r="D55" s="32"/>
       <c r="E55" s="32"/>
@@ -1594,12 +1553,11 @@
       <c r="H55" s="32"/>
       <c r="I55" s="33"/>
       <c r="J55" s="33"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="30"/>
-    </row>
-    <row r="56" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K55" s="30"/>
+    </row>
+    <row r="56" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
-      <c r="B56" s="32"/>
+      <c r="B56" s="18"/>
       <c r="C56" s="32"/>
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
@@ -1608,10 +1566,9 @@
       <c r="H56" s="18"/>
       <c r="I56" s="31"/>
       <c r="J56" s="20"/>
-      <c r="K56" s="32"/>
-      <c r="L56" s="30"/>
-    </row>
-    <row r="57" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K56" s="30"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
       <c r="B57" s="18"/>
       <c r="C57" s="32"/>
@@ -1622,10 +1579,9 @@
       <c r="H57" s="18"/>
       <c r="I57" s="31"/>
       <c r="J57" s="20"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="30"/>
-    </row>
-    <row r="58" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K57" s="30"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="18"/>
       <c r="B58" s="18"/>
       <c r="C58" s="32"/>
@@ -1636,10 +1592,9 @@
       <c r="H58" s="18"/>
       <c r="I58" s="31"/>
       <c r="J58" s="20"/>
-      <c r="K58" s="32"/>
-      <c r="L58" s="30"/>
-    </row>
-    <row r="59" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K58" s="30"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="18"/>
       <c r="C59" s="32"/>
@@ -1650,12 +1605,11 @@
       <c r="H59" s="18"/>
       <c r="I59" s="31"/>
       <c r="J59" s="20"/>
-      <c r="K59" s="32"/>
-      <c r="L59" s="30"/>
-    </row>
-    <row r="60" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K59" s="30"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
-      <c r="B60" s="18"/>
+      <c r="B60" s="32"/>
       <c r="C60" s="32"/>
       <c r="D60" s="32"/>
       <c r="E60" s="32"/>
@@ -1664,12 +1618,11 @@
       <c r="H60" s="32"/>
       <c r="I60" s="33"/>
       <c r="J60" s="33"/>
-      <c r="K60" s="32"/>
-      <c r="L60" s="30"/>
-    </row>
-    <row r="61" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K60" s="30"/>
+    </row>
+    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
-      <c r="B61" s="32"/>
+      <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -1677,13 +1630,12 @@
       <c r="G61" s="31"/>
       <c r="H61" s="18"/>
       <c r="I61" s="29"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="30"/>
-    </row>
-    <row r="62" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J61" s="8"/>
+      <c r="K61" s="30"/>
+    </row>
+    <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
-      <c r="B62" s="5"/>
+      <c r="B62" s="18"/>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
@@ -1692,17 +1644,11 @@
       <c r="H62" s="18"/>
       <c r="I62" s="29"/>
       <c r="J62" s="29"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="30"/>
-    </row>
-    <row r="63" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B63" s="18"/>
+      <c r="K62" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="J48:K48"/>
+  <mergeCells count="1">
+    <mergeCell ref="A3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
minor excel template change
</commit_message>
<xml_diff>
--- a/app/files/Part-Time Lecturer Requisition Form - template new.xlsx
+++ b/app/files/Part-Time Lecturer Requisition Form - template new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\k\Main\Capstone Project\CoursePDF Extractor\Capstone-Project\app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA99279-8C82-4A9E-8EF1-885ADB493410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB6D295-8C5F-4FC3-91B4-080252739364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -301,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -480,24 +480,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC6C6C6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -606,9 +593,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -926,7 +910,7 @@
   <dimension ref="A3:K62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -945,19 +929,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="46"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -1159,8 +1143,7 @@
       <c r="H20" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="45">
+      <c r="I20" s="44">
         <f>D20*G20</f>
         <v>0</v>
       </c>

</xml_diff>